<commit_message>
result of check for kf_sphere_vaidity.pptm Works fine.
</commit_message>
<xml_diff>
--- a/FeScienceTimingLogBook2024-2025.xlsx
+++ b/FeScienceTimingLogBook2024-2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SHARE\Fe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A44F60-D7B0-465A-AF46-B8A3CB84903C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497D6E7E-5EEE-4222-8543-77091BE4DAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="0" windowWidth="20360" windowHeight="20970" xr2:uid="{90053488-A26B-4176-8F88-FB9A8AF34211}"/>
+    <workbookView xWindow="5780" yWindow="0" windowWidth="22720" windowHeight="20970" xr2:uid="{90053488-A26B-4176-8F88-FB9A8AF34211}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
   <si>
     <t xml:space="preserve">Bug fixing; Attempt to downgrate </t>
   </si>
@@ -90,13 +90,31 @@
   </si>
   <si>
     <t>kf_sphere/PageOp</t>
+  </si>
+  <si>
+    <t>kf_sphere/PageOp 0.5</t>
+  </si>
+  <si>
+    <t>saveobj description &amp; L&amp;D</t>
+  </si>
+  <si>
+    <t>saveobj description 0.5</t>
+  </si>
+  <si>
+    <t>(hospital)</t>
+  </si>
+  <si>
+    <t>Test euphonic 0.5</t>
+  </si>
+  <si>
+    <t>(Matlab issues)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +139,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,7 +200,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -185,6 +209,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -522,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F03AC02-A4F3-4CAA-9F06-946DEB4C63C4}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29:H29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -803,7 +828,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45612</v>
       </c>
@@ -820,7 +845,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45613</v>
       </c>
@@ -837,7 +862,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45614</v>
       </c>
@@ -854,7 +879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45615</v>
       </c>
@@ -871,7 +896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45616</v>
       </c>
@@ -888,7 +913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45617</v>
       </c>
@@ -905,7 +930,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>45618</v>
       </c>
@@ -922,7 +947,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45619</v>
       </c>
@@ -939,7 +964,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>45620</v>
       </c>
@@ -956,7 +981,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>45621</v>
       </c>
@@ -976,7 +1001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>45622</v>
       </c>
@@ -997,7 +1022,7 @@
       </c>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>45623</v>
       </c>
@@ -1017,7 +1042,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45624</v>
       </c>
@@ -1034,10 +1059,10 @@
         <v>45685</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>45625</v>
       </c>
@@ -1053,8 +1078,11 @@
       <c r="F30" s="2">
         <v>45686</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G30" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>45626</v>
       </c>
@@ -1070,8 +1098,14 @@
       <c r="F31" s="2">
         <v>45687</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G31" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C32" s="2">
         <v>45657</v>
       </c>
@@ -1080,6 +1114,12 @@
       </c>
       <c r="F32" s="2">
         <v>45688</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
minor changes to cylindrical background removal script accounting for latest Horace development.
</commit_message>
<xml_diff>
--- a/FeScienceTimingLogBook2024-2025.xlsx
+++ b/FeScienceTimingLogBook2024-2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SHARE\Fe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497D6E7E-5EEE-4222-8543-77091BE4DAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B803F2-7B44-44F9-866D-8A2E54C2B118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="0" windowWidth="22720" windowHeight="20970" xr2:uid="{90053488-A26B-4176-8F88-FB9A8AF34211}"/>
+    <workbookView xWindow="7240" yWindow="2880" windowWidth="28800" windowHeight="15450" xr2:uid="{90053488-A26B-4176-8F88-FB9A8AF34211}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="39">
   <si>
     <t xml:space="preserve">Bug fixing; Attempt to downgrate </t>
   </si>
@@ -89,12 +89,6 @@
     <t>kf_sphere_0.5</t>
   </si>
   <si>
-    <t>kf_sphere/PageOp</t>
-  </si>
-  <si>
-    <t>kf_sphere/PageOp 0.5</t>
-  </si>
-  <si>
     <t>saveobj description &amp; L&amp;D</t>
   </si>
   <si>
@@ -108,13 +102,83 @@
   </si>
   <si>
     <t>(Matlab issues)</t>
+  </si>
+  <si>
+    <t>Matlab issues &amp;sof_qw2</t>
+  </si>
+  <si>
+    <t>fast map</t>
+  </si>
+  <si>
+    <t>OPEN DAY</t>
+  </si>
+  <si>
+    <t>fast map/Jacob's inheritance</t>
+  </si>
+  <si>
+    <t>fast map &amp;calc_qw_pix2</t>
+  </si>
+  <si>
+    <t>calc_qw_pix2</t>
+  </si>
+  <si>
+    <t>presentation</t>
+  </si>
+  <si>
+    <t>kf_sphere/background</t>
+  </si>
+  <si>
+    <t>presentations/discussions</t>
+  </si>
+  <si>
+    <t>calc_qw_pix2/calc_all_pixels</t>
+  </si>
+  <si>
+    <t>sqw_op as contribution 0.5 &amp; L&amp;D</t>
+  </si>
+  <si>
+    <t>kf_sphere/PageOp-sqw_op</t>
+  </si>
+  <si>
+    <t>kf_sphere/PageOp-sqw_op 0.5</t>
+  </si>
+  <si>
+    <t>sqw_op</t>
+  </si>
+  <si>
+    <t>APR</t>
+  </si>
+  <si>
+    <t>kf_sphere=&gt;instrument_view</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.5Boothroid;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -&gt; 0.5Instrument_view</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,8 +213,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +255,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -200,7 +277,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -210,6 +287,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -547,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F03AC02-A4F3-4CAA-9F06-946DEB4C63C4}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -560,9 +640,13 @@
     <col min="3" max="3" width="12.26953125" customWidth="1"/>
     <col min="5" max="5" width="20.08984375" customWidth="1"/>
     <col min="6" max="6" width="13.36328125" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.453125" customWidth="1"/>
+    <col min="18" max="19" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>45597</v>
       </c>
@@ -572,8 +656,17 @@
       <c r="F1" s="1">
         <v>45658</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K1" s="1">
+        <v>45689</v>
+      </c>
+      <c r="O1" s="1">
+        <v>45717</v>
+      </c>
+      <c r="R1" s="1">
+        <v>45748</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45597</v>
       </c>
@@ -589,8 +682,23 @@
       <c r="G2" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K2" s="2">
+        <v>45689</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="2">
+        <v>45717</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="2">
+        <v>45748</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45598</v>
       </c>
@@ -606,8 +714,20 @@
       <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K3" s="2">
+        <v>45690</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="2">
+        <v>45718</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45599</v>
       </c>
@@ -623,8 +743,20 @@
       <c r="G4" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K4" s="2">
+        <v>45691</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="2">
+        <v>45719</v>
+      </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45600</v>
       </c>
@@ -640,8 +772,20 @@
       <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K5" s="2">
+        <v>45692</v>
+      </c>
+      <c r="L5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="2">
+        <v>45720</v>
+      </c>
+      <c r="P5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45601</v>
       </c>
@@ -657,8 +801,20 @@
       <c r="G6" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K6" s="2">
+        <v>45693</v>
+      </c>
+      <c r="L6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="2">
+        <v>45721</v>
+      </c>
+      <c r="P6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45602</v>
       </c>
@@ -674,8 +830,20 @@
       <c r="G7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K7" s="2">
+        <v>45694</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" s="2">
+        <v>45722</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45603</v>
       </c>
@@ -691,8 +859,20 @@
       <c r="G8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K8" s="2">
+        <v>45695</v>
+      </c>
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="2">
+        <v>45723</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45604</v>
       </c>
@@ -708,8 +888,20 @@
       <c r="G9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K9" s="2">
+        <v>45696</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9" s="2">
+        <v>45724</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45605</v>
       </c>
@@ -725,8 +917,20 @@
       <c r="G10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K10" s="2">
+        <v>45697</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O10" s="2">
+        <v>45725</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45606</v>
       </c>
@@ -742,8 +946,20 @@
       <c r="G11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K11" s="2">
+        <v>45698</v>
+      </c>
+      <c r="L11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="2">
+        <v>45726</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45607</v>
       </c>
@@ -759,8 +975,20 @@
       <c r="G12" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K12" s="2">
+        <v>45699</v>
+      </c>
+      <c r="L12" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="2">
+        <v>45727</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45608</v>
       </c>
@@ -776,8 +1004,20 @@
       <c r="G13" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K13" s="2">
+        <v>45700</v>
+      </c>
+      <c r="L13" t="s">
+        <v>26</v>
+      </c>
+      <c r="O13" s="2">
+        <v>45728</v>
+      </c>
+      <c r="P13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45609</v>
       </c>
@@ -793,8 +1033,20 @@
       <c r="G14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K14" s="2">
+        <v>45701</v>
+      </c>
+      <c r="L14" t="s">
+        <v>26</v>
+      </c>
+      <c r="O14" s="2">
+        <v>45729</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>45610</v>
       </c>
@@ -810,8 +1062,20 @@
       <c r="G15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K15" s="2">
+        <v>45702</v>
+      </c>
+      <c r="L15" t="s">
+        <v>26</v>
+      </c>
+      <c r="O15" s="2">
+        <v>45730</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45611</v>
       </c>
@@ -827,8 +1091,20 @@
       <c r="G16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K16" s="2">
+        <v>45703</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O16" s="2">
+        <v>45731</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45612</v>
       </c>
@@ -844,8 +1120,20 @@
       <c r="G17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K17" s="2">
+        <v>45704</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O17" s="2">
+        <v>45732</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45613</v>
       </c>
@@ -861,8 +1149,20 @@
       <c r="G18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K18" s="2">
+        <v>45705</v>
+      </c>
+      <c r="L18" t="s">
+        <v>26</v>
+      </c>
+      <c r="O18" s="2">
+        <v>45733</v>
+      </c>
+      <c r="P18" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45614</v>
       </c>
@@ -878,8 +1178,20 @@
       <c r="G19" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K19" s="2">
+        <v>45706</v>
+      </c>
+      <c r="L19" t="s">
+        <v>26</v>
+      </c>
+      <c r="O19" s="2">
+        <v>45734</v>
+      </c>
+      <c r="P19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45615</v>
       </c>
@@ -895,8 +1207,20 @@
       <c r="G20" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K20" s="2">
+        <v>45707</v>
+      </c>
+      <c r="L20" t="s">
+        <v>26</v>
+      </c>
+      <c r="O20" s="2">
+        <v>45735</v>
+      </c>
+      <c r="P20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45616</v>
       </c>
@@ -912,8 +1236,20 @@
       <c r="G21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K21" s="2">
+        <v>45708</v>
+      </c>
+      <c r="L21" t="s">
+        <v>27</v>
+      </c>
+      <c r="O21" s="2">
+        <v>45736</v>
+      </c>
+      <c r="P21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45617</v>
       </c>
@@ -929,8 +1265,20 @@
       <c r="G22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K22" s="2">
+        <v>45709</v>
+      </c>
+      <c r="L22" t="s">
+        <v>27</v>
+      </c>
+      <c r="O22" s="2">
+        <v>45737</v>
+      </c>
+      <c r="P22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>45618</v>
       </c>
@@ -946,8 +1294,20 @@
       <c r="G23" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K23" s="2">
+        <v>45710</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O23" s="2">
+        <v>45738</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45619</v>
       </c>
@@ -963,8 +1323,20 @@
       <c r="G24" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K24" s="2">
+        <v>45711</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O24" s="2">
+        <v>45739</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>45620</v>
       </c>
@@ -980,8 +1352,20 @@
       <c r="G25" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K25" s="2">
+        <v>45712</v>
+      </c>
+      <c r="L25" t="s">
+        <v>28</v>
+      </c>
+      <c r="O25" s="2">
+        <v>45740</v>
+      </c>
+      <c r="P25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>45621</v>
       </c>
@@ -1000,8 +1384,20 @@
       <c r="G26" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K26" s="2">
+        <v>45713</v>
+      </c>
+      <c r="L26" t="s">
+        <v>28</v>
+      </c>
+      <c r="O26" s="2">
+        <v>45741</v>
+      </c>
+      <c r="P26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>45622</v>
       </c>
@@ -1017,12 +1413,24 @@
       <c r="F27" s="2">
         <v>45683</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K27" s="2">
+        <v>45714</v>
+      </c>
+      <c r="L27" t="s">
+        <v>28</v>
+      </c>
+      <c r="O27" s="2">
+        <v>45742</v>
+      </c>
+      <c r="P27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>45623</v>
       </c>
@@ -1039,10 +1447,22 @@
         <v>45684</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="K28" s="2">
+        <v>45715</v>
+      </c>
+      <c r="L28" t="s">
+        <v>27</v>
+      </c>
+      <c r="O28" s="2">
+        <v>45743</v>
+      </c>
+      <c r="P28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45624</v>
       </c>
@@ -1059,10 +1479,19 @@
         <v>45685</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="K29" s="2">
+        <v>45716</v>
+      </c>
+      <c r="L29" t="s">
+        <v>27</v>
+      </c>
+      <c r="O29" s="2">
+        <v>45744</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>45625</v>
       </c>
@@ -1079,10 +1508,17 @@
         <v>45686</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="K30" s="2"/>
+      <c r="O30" s="2">
+        <v>45745</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>45626</v>
       </c>
@@ -1099,13 +1535,19 @@
         <v>45687</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="O31" s="2">
+        <v>45746</v>
+      </c>
+      <c r="P31" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C32" s="2">
         <v>45657</v>
       </c>
@@ -1116,10 +1558,13 @@
         <v>45688</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I32" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="O32" s="2">
+        <v>45747</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
attempt to build 4D background something promising but strange
</commit_message>
<xml_diff>
--- a/FeScienceTimingLogBook2024-2025.xlsx
+++ b/FeScienceTimingLogBook2024-2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SHARE\Fe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B803F2-7B44-44F9-866D-8A2E54C2B118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07740F61-FFD5-449B-8B2E-D6336666B383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="2880" windowWidth="28800" windowHeight="15450" xr2:uid="{90053488-A26B-4176-8F88-FB9A8AF34211}"/>
+    <workbookView xWindow="50" yWindow="350" windowWidth="38440" windowHeight="20620" xr2:uid="{90053488-A26B-4176-8F88-FB9A8AF34211}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="44">
   <si>
     <t xml:space="preserve">Bug fixing; Attempt to downgrate </t>
   </si>
@@ -172,6 +172,40 @@
       </rPr>
       <t xml:space="preserve"> -&gt; 0.5Instrument_view</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.5Boothroid;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -&gt; 0.5review</t>
+    </r>
+  </si>
+  <si>
+    <t>Symop</t>
+  </si>
+  <si>
+    <t>Symop/Admin</t>
+  </si>
+  <si>
+    <t>Instrument_view_cut Documentation</t>
+  </si>
+  <si>
+    <t>parallel framework + L&amp;D</t>
   </si>
 </sst>
 </file>
@@ -627,16 +661,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F03AC02-A4F3-4CAA-9F06-946DEB4C63C4}">
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="2" max="2" width="22.7265625" customWidth="1"/>
     <col min="3" max="3" width="12.26953125" customWidth="1"/>
     <col min="5" max="5" width="20.08984375" customWidth="1"/>
     <col min="6" max="6" width="13.36328125" customWidth="1"/>
@@ -646,7 +680,7 @@
     <col min="18" max="19" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>45597</v>
       </c>
@@ -662,11 +696,8 @@
       <c r="O1" s="1">
         <v>45717</v>
       </c>
-      <c r="R1" s="1">
-        <v>45748</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45597</v>
       </c>
@@ -694,11 +725,8 @@
       <c r="P2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="2">
-        <v>45748</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45598</v>
       </c>
@@ -727,7 +755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45599</v>
       </c>
@@ -756,7 +784,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45600</v>
       </c>
@@ -785,7 +813,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45601</v>
       </c>
@@ -814,7 +842,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45602</v>
       </c>
@@ -843,7 +871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45603</v>
       </c>
@@ -872,7 +900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45604</v>
       </c>
@@ -901,7 +929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45605</v>
       </c>
@@ -930,7 +958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45606</v>
       </c>
@@ -959,7 +987,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45607</v>
       </c>
@@ -988,7 +1016,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45608</v>
       </c>
@@ -1017,7 +1045,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45609</v>
       </c>
@@ -1046,7 +1074,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>45610</v>
       </c>
@@ -1075,7 +1103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45611</v>
       </c>
@@ -1490,6 +1518,9 @@
       <c r="O29" s="2">
         <v>45744</v>
       </c>
+      <c r="P29" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
@@ -1566,9 +1597,314 @@
       <c r="O32" s="2">
         <v>45747</v>
       </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="P32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C33" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>45748</v>
+      </c>
+      <c r="C35" s="1">
+        <v>45778</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>45748</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="2">
+        <v>45778</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>45749</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="2">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>45750</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="2">
+        <v>45780</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>45751</v>
+      </c>
+      <c r="C39" s="2">
+        <v>45781</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>45752</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>45753</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="2">
+        <v>45783</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>45754</v>
+      </c>
+      <c r="C42" s="2">
+        <v>45784</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="2">
+        <v>45755</v>
+      </c>
+      <c r="C43" s="2">
+        <v>45785</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="2">
+        <v>45756</v>
+      </c>
+      <c r="C44" s="2">
+        <v>45786</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>45757</v>
+      </c>
+      <c r="C45" s="2">
+        <v>45787</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="2">
+        <v>45758</v>
+      </c>
+      <c r="C46" s="2">
+        <v>45788</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="2">
+        <v>45759</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="2">
+        <v>45789</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>45760</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="2">
+        <v>45790</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="2">
+        <v>45761</v>
+      </c>
+      <c r="C49" s="2">
+        <v>45791</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="2">
+        <v>45762</v>
+      </c>
+      <c r="C50" s="2">
+        <v>45792</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="2">
+        <v>45763</v>
+      </c>
+      <c r="C51" s="2">
+        <v>45793</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="2">
+        <v>45764</v>
+      </c>
+      <c r="C52" s="2">
+        <v>45794</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="2">
+        <v>45765</v>
+      </c>
+      <c r="C53" s="2">
+        <v>45795</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="2">
+        <v>45766</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="2">
+        <v>45796</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="2">
+        <v>45767</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="2">
+        <v>45797</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="2">
+        <v>45768</v>
+      </c>
+      <c r="C56" s="2">
+        <v>45798</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="2">
+        <v>45769</v>
+      </c>
+      <c r="C57" s="2">
+        <v>45799</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="2">
+        <v>45770</v>
+      </c>
+      <c r="C58" s="2">
+        <v>45800</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="2">
+        <v>45771</v>
+      </c>
+      <c r="C59" s="2">
+        <v>45801</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="2">
+        <v>45772</v>
+      </c>
+      <c r="C60" s="2">
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="2">
+        <v>45773</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" s="2">
+        <v>45803</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="2">
+        <v>45774</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="2">
+        <v>45804</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="2">
+        <v>45775</v>
+      </c>
+      <c r="C63" s="2">
+        <v>45805</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="2">
+        <v>45776</v>
+      </c>
+      <c r="C64" s="2">
+        <v>45806</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="2">
+        <v>45777</v>
+      </c>
+      <c r="C65" s="2">
+        <v>45807</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" s="2"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="2"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="2"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" s="2"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Test script to remove background which shows that background removal does not work
</commit_message>
<xml_diff>
--- a/FeScienceTimingLogBook2024-2025.xlsx
+++ b/FeScienceTimingLogBook2024-2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SHARE\Fe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07740F61-FFD5-449B-8B2E-D6336666B383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A376CAB-1CEE-47BF-B345-2E0DE5A00441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50" yWindow="350" windowWidth="38440" windowHeight="20620" xr2:uid="{90053488-A26B-4176-8F88-FB9A8AF34211}"/>
+    <workbookView xWindow="1150" yWindow="1570" windowWidth="27400" windowHeight="17270" xr2:uid="{90053488-A26B-4176-8F88-FB9A8AF34211}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="48">
   <si>
     <t xml:space="preserve">Bug fixing; Attempt to downgrate </t>
   </si>
@@ -206,6 +206,18 @@
   </si>
   <si>
     <t>parallel framework + L&amp;D</t>
+  </si>
+  <si>
+    <t>background calc</t>
+  </si>
+  <si>
+    <t>-nopix in sqw_op</t>
+  </si>
+  <si>
+    <t>sqw_op_bin_pixels</t>
+  </si>
+  <si>
+    <t>APR/sqw_op_bin_pixels</t>
   </si>
 </sst>
 </file>
@@ -255,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +307,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -311,7 +329,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -324,6 +342,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -663,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F03AC02-A4F3-4CAA-9F06-946DEB4C63C4}">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1652,6 +1673,9 @@
       <c r="A39" s="2">
         <v>45751</v>
       </c>
+      <c r="B39" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="C39" s="2">
         <v>45781</v>
       </c>
@@ -1685,6 +1709,9 @@
       <c r="A42" s="2">
         <v>45754</v>
       </c>
+      <c r="B42" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="C42" s="2">
         <v>45784</v>
       </c>
@@ -1693,6 +1720,9 @@
       <c r="A43" s="2">
         <v>45755</v>
       </c>
+      <c r="B43" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="C43" s="2">
         <v>45785</v>
       </c>
@@ -1701,6 +1731,9 @@
       <c r="A44" s="2">
         <v>45756</v>
       </c>
+      <c r="B44" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="C44" s="2">
         <v>45786</v>
       </c>
@@ -1709,6 +1742,9 @@
       <c r="A45" s="2">
         <v>45757</v>
       </c>
+      <c r="B45" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="C45" s="2">
         <v>45787</v>
       </c>
@@ -1717,6 +1753,9 @@
       <c r="A46" s="2">
         <v>45758</v>
       </c>
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
       <c r="C46" s="2">
         <v>45788</v>
       </c>
@@ -1747,6 +1786,9 @@
       <c r="A49" s="2">
         <v>45761</v>
       </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
       <c r="C49" s="2">
         <v>45791</v>
       </c>
@@ -1754,6 +1796,9 @@
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>45762</v>
+      </c>
+      <c r="B50" t="s">
+        <v>46</v>
       </c>
       <c r="C50" s="2">
         <v>45792</v>

</xml_diff>

<commit_message>
various background analysis routines
</commit_message>
<xml_diff>
--- a/FeScienceTimingLogBook2024-2025.xlsx
+++ b/FeScienceTimingLogBook2024-2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SHARE\Fe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A376CAB-1CEE-47BF-B345-2E0DE5A00441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E772490-620B-4F22-A4E4-2B95375A1A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1150" yWindow="1570" windowWidth="27400" windowHeight="17270" xr2:uid="{90053488-A26B-4176-8F88-FB9A8AF34211}"/>
+    <workbookView xWindow="750" yWindow="1330" windowWidth="28800" windowHeight="15450" xr2:uid="{90053488-A26B-4176-8F88-FB9A8AF34211}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="48">
   <si>
     <t xml:space="preserve">Bug fixing; Attempt to downgrate </t>
   </si>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F03AC02-A4F3-4CAA-9F06-946DEB4C63C4}">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1808,6 +1808,9 @@
       <c r="A51" s="2">
         <v>45763</v>
       </c>
+      <c r="B51" t="s">
+        <v>46</v>
+      </c>
       <c r="C51" s="2">
         <v>45793</v>
       </c>
@@ -1816,6 +1819,9 @@
       <c r="A52" s="2">
         <v>45764</v>
       </c>
+      <c r="B52" t="s">
+        <v>46</v>
+      </c>
       <c r="C52" s="2">
         <v>45794</v>
       </c>
@@ -1824,6 +1830,9 @@
       <c r="A53" s="2">
         <v>45765</v>
       </c>
+      <c r="B53" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="C53" s="2">
         <v>45795</v>
       </c>
@@ -1854,6 +1863,9 @@
       <c r="A56" s="2">
         <v>45768</v>
       </c>
+      <c r="B56" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="C56" s="2">
         <v>45798</v>
       </c>
@@ -1862,6 +1874,9 @@
       <c r="A57" s="2">
         <v>45769</v>
       </c>
+      <c r="B57" t="s">
+        <v>46</v>
+      </c>
       <c r="C57" s="2">
         <v>45799</v>
       </c>
@@ -1870,6 +1885,9 @@
       <c r="A58" s="2">
         <v>45770</v>
       </c>
+      <c r="B58" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="C58" s="2">
         <v>45800</v>
       </c>
@@ -1878,6 +1896,9 @@
       <c r="A59" s="2">
         <v>45771</v>
       </c>
+      <c r="B59" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="C59" s="2">
         <v>45801</v>
       </c>
@@ -1886,6 +1907,9 @@
       <c r="A60" s="2">
         <v>45772</v>
       </c>
+      <c r="B60" t="s">
+        <v>47</v>
+      </c>
       <c r="C60" s="2">
         <v>45802</v>
       </c>
@@ -1915,6 +1939,9 @@
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>45775</v>
+      </c>
+      <c r="B63" t="s">
+        <v>46</v>
       </c>
       <c r="C63" s="2">
         <v>45805</v>

</xml_diff>

<commit_message>
moved all to first Brilluoin zone. Background removal for 400meV and various file transformations
</commit_message>
<xml_diff>
--- a/FeScienceTimingLogBook2024-2025.xlsx
+++ b/FeScienceTimingLogBook2024-2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SHARE\Fe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E772490-620B-4F22-A4E4-2B95375A1A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A87DDC-4C8C-454C-8DC3-F94FDBFFA8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="750" yWindow="1330" windowWidth="28800" windowHeight="15450" xr2:uid="{90053488-A26B-4176-8F88-FB9A8AF34211}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="58">
   <si>
     <t xml:space="preserve">Bug fixing; Attempt to downgrate </t>
   </si>
@@ -218,6 +218,36 @@
   </si>
   <si>
     <t>APR/sqw_op_bin_pixels</t>
+  </si>
+  <si>
+    <t>magneticFF</t>
+  </si>
+  <si>
+    <t>backgroun&amp;Symmetry calc</t>
+  </si>
+  <si>
+    <t>EH</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>magneticFF/sqw_op+bin</t>
+  </si>
+  <si>
+    <t>pixel cahce</t>
+  </si>
+  <si>
+    <t>pixel cahce/plotting review</t>
+  </si>
+  <si>
+    <t>-combine in sqw_op</t>
+  </si>
+  <si>
+    <t>background/symmetry calc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">combine/test interdependencies </t>
   </si>
 </sst>
 </file>
@@ -684,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F03AC02-A4F3-4CAA-9F06-946DEB4C63C4}">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1643,6 +1673,9 @@
       <c r="C36" s="2">
         <v>45778</v>
       </c>
+      <c r="D36" s="14" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
@@ -1654,6 +1687,9 @@
       <c r="C37" s="2">
         <v>45779</v>
       </c>
+      <c r="D37" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
@@ -1693,6 +1729,9 @@
       <c r="C40" s="2">
         <v>45782</v>
       </c>
+      <c r="D40" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
@@ -1704,6 +1743,9 @@
       <c r="C41" s="2">
         <v>45783</v>
       </c>
+      <c r="D41" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
@@ -1715,6 +1757,9 @@
       <c r="C42" s="2">
         <v>45784</v>
       </c>
+      <c r="D42" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
@@ -1726,6 +1771,9 @@
       <c r="C43" s="2">
         <v>45785</v>
       </c>
+      <c r="D43" s="14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
@@ -1737,6 +1785,9 @@
       <c r="C44" s="2">
         <v>45786</v>
       </c>
+      <c r="D44" s="14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
@@ -1748,6 +1799,9 @@
       <c r="C45" s="2">
         <v>45787</v>
       </c>
+      <c r="D45" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
@@ -1759,6 +1813,9 @@
       <c r="C46" s="2">
         <v>45788</v>
       </c>
+      <c r="D46" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
@@ -1770,6 +1827,9 @@
       <c r="C47" s="2">
         <v>45789</v>
       </c>
+      <c r="D47" s="14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
@@ -1781,8 +1841,11 @@
       <c r="C48" s="2">
         <v>45790</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D48" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>45761</v>
       </c>
@@ -1792,8 +1855,11 @@
       <c r="C49" s="2">
         <v>45791</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D49" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>45762</v>
       </c>
@@ -1803,8 +1869,11 @@
       <c r="C50" s="2">
         <v>45792</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D50" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>45763</v>
       </c>
@@ -1814,8 +1883,11 @@
       <c r="C51" s="2">
         <v>45793</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D51" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>45764</v>
       </c>
@@ -1825,19 +1897,25 @@
       <c r="C52" s="2">
         <v>45794</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D52" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>45765</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="C53" s="2">
         <v>45795</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D53" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>45766</v>
       </c>
@@ -1848,7 +1926,7 @@
         <v>45796</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>45767</v>
       </c>
@@ -1859,18 +1937,18 @@
         <v>45797</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>45768</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="C56" s="2">
         <v>45798</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>45769</v>
       </c>
@@ -1881,7 +1959,7 @@
         <v>45799</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>45770</v>
       </c>
@@ -1892,7 +1970,7 @@
         <v>45800</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>45771</v>
       </c>
@@ -1902,8 +1980,11 @@
       <c r="C59" s="2">
         <v>45801</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D59" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>45772</v>
       </c>
@@ -1913,8 +1994,11 @@
       <c r="C60" s="2">
         <v>45802</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D60" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>45773</v>
       </c>
@@ -1925,7 +2009,7 @@
         <v>45803</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>45774</v>
       </c>
@@ -1936,7 +2020,7 @@
         <v>45804</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>45775</v>
       </c>
@@ -1947,9 +2031,12 @@
         <v>45805</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>45776</v>
+      </c>
+      <c r="B64" t="s">
+        <v>46</v>
       </c>
       <c r="C64" s="2">
         <v>45806</v>
@@ -1958,6 +2045,9 @@
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>45777</v>
+      </c>
+      <c r="B65" t="s">
+        <v>48</v>
       </c>
       <c r="C65" s="2">
         <v>45807</v>

</xml_diff>

<commit_message>
preliminary results for comparison with Jerome theory. Does not look good
</commit_message>
<xml_diff>
--- a/FeScienceTimingLogBook2024-2025.xlsx
+++ b/FeScienceTimingLogBook2024-2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SHARE\Fe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A87DDC-4C8C-454C-8DC3-F94FDBFFA8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E32C5C-52CD-4384-BB3F-2413B10A292D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="750" yWindow="1330" windowWidth="28800" windowHeight="15450" xr2:uid="{90053488-A26B-4176-8F88-FB9A8AF34211}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="59">
   <si>
     <t xml:space="preserve">Bug fixing; Attempt to downgrate </t>
   </si>
@@ -249,12 +249,15 @@
   <si>
     <t xml:space="preserve">combine/test interdependencies </t>
   </si>
+  <si>
+    <t>mex in cuts</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,6 +295,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -359,7 +369,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -375,6 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -715,7 +726,7 @@
   <dimension ref="A1:P71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1925,6 +1936,9 @@
       <c r="C54" s="2">
         <v>45796</v>
       </c>
+      <c r="D54" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
@@ -1936,6 +1950,9 @@
       <c r="C55" s="2">
         <v>45797</v>
       </c>
+      <c r="D55" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
@@ -1947,6 +1964,9 @@
       <c r="C56" s="2">
         <v>45798</v>
       </c>
+      <c r="D56" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
@@ -1958,6 +1978,9 @@
       <c r="C57" s="2">
         <v>45799</v>
       </c>
+      <c r="D57" s="13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
@@ -1969,6 +1992,9 @@
       <c r="C58" s="2">
         <v>45800</v>
       </c>
+      <c r="D58" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
@@ -2008,6 +2034,9 @@
       <c r="C61" s="2">
         <v>45803</v>
       </c>
+      <c r="D61" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
@@ -2019,6 +2048,9 @@
       <c r="C62" s="2">
         <v>45804</v>
       </c>
+      <c r="D62" s="15" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
@@ -2030,6 +2062,9 @@
       <c r="C63" s="2">
         <v>45805</v>
       </c>
+      <c r="D63" s="15" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
@@ -2041,8 +2076,11 @@
       <c r="C64" s="2">
         <v>45806</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D64" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>45777</v>
       </c>
@@ -2052,20 +2090,23 @@
       <c r="C65" s="2">
         <v>45807</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D65" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="2"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="2"/>
     </row>
   </sheetData>

</xml_diff>